<commit_message>
Project Euler Q 0021-0030
</commit_message>
<xml_diff>
--- a/Document/ProjectEuler.xlsx
+++ b/Document/ProjectEuler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="580" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="570" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
   <si>
     <t>ProblemIndex</t>
   </si>
@@ -626,13 +626,1207 @@
 소수점 아래 n번째 숫자를 dn이라고 했을 때, 아래 식의 값은 얼마입니까?
   d1 × d10 × d100 × d1000 × d10000 × d100000 × d1000000 </t>
   </si>
+  <si>
+    <r>
+      <t>41</t>
+    </r>
+  </si>
+  <si>
+    <t>n자리 팬디지털 소수 중에서 가장 큰 수</t>
+  </si>
+  <si>
+    <t>1부터 n까지의 숫자를 하나씩만 써서 만든 n자리 숫자를 팬디지털(pandigital)이라고 부릅니다.
+2143은 4자리 팬디지털인데, 이 수는 동시에 소수이기도 합니다.
+n자리 팬디지털 소수 중에서 가장 큰 수는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>42</t>
+    </r>
+  </si>
+  <si>
+    <t>주어진 텍스트 파일에 들어있는 '삼각단어'의 개수는?</t>
+  </si>
+  <si>
+    <t>n번째 삼각수는 tn = ½ n (n + 1) 이라는 식으로 구할 수 있는데, 처음 10개는 아래와 같습니다.
+  1, 3, 6, 10, 15, 21, 28, 36, 45, 55, ...
+어떤 영어 단어에 대해서, 각 철자의 알파벳 순서(A=1, B=2, ..., Z=26)를 모두 더한 값을 '단어값'이라 부르기로 합니다. 예를 들어 'SKY'의 단어값은 19 + 11 + 25 = 55가 되는데, 이것은 우연히도 t10과 같습니다.
+이렇게 어떤 단어의 단어값이 삼각수일 경우에는 이 단어를 '삼각단어'라 부르기로 합니다.
+약 16KB의 텍스트 파일 words.txt에는 2000개 정도의 영어 단어가 수록되어 있습니다. 이 중에서 삼각단어는 모두 몇 개입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>43</t>
+    </r>
+  </si>
+  <si>
+    <t>부분열에 관련된 특이한 성질을 가진 모든 팬디지털 숫자의 합</t>
+  </si>
+  <si>
+    <t>숫자 1406357289은 0 ~ 9 팬디지털인데, 부분열에 관련된 재미있는 성질을 가지고 있습니다.
+d1을 첫째 자리수, d2를 둘째 자리수...라고 했을 때, 다음과 같은 사실을 발견할 수 있습니다.
+  •d2 d3 d4 = 406 → 2로 나누어 떨어짐
+  •d3 d4 d5 = 063 → 3으로 나누어 떨어짐
+  •d4 d5 d6 = 635 → 5로 나누어 떨어짐
+  •d5 d6 d7 = 357 → 7로 나누어 떨어짐
+  •d6 d7 d8 = 572 → 11로 나누어 떨어짐
+  •d7 d8 d9 = 728 → 13으로 나누어 떨어짐
+  •d8 d9 d10 = 289 → 17로 나누어 떨어짐
+위와 같은 성질을 갖는 0 ~ 9 팬디지털을 모두 찾아서 그 합을 구하면 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>44</t>
+    </r>
+  </si>
+  <si>
+    <t>합과 차도 모두 오각수인 두 오각수 차의 최소값은?</t>
+  </si>
+  <si>
+    <t>오각수는 Pn = n (3n − 1)/2 라는 공식으로 구할 수 있고, 처음 10개의 오각수는 다음과 같습니다.
+  1, 5, 12, 22, 35, 51, 70, 92, 117, 145, ...
+위에서 P4 + P7 = 22 + 70 = 92 = P8이 됨을 볼 수 있습니다. 하지만 두 값의 차인 70 − 22 = 48 은 오각수가 아닙니다.
+합과 차도 모두 오각수인 두 오각수 Pj, Pk 에 대해서, 그 차이 D = | Pk − Pj |  는 가장 작을 때 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>45</t>
+    </r>
+  </si>
+  <si>
+    <t>오각수와 육각수도 되는, 40755 다음으로 큰 삼각수는?</t>
+  </si>
+  <si>
+    <t>삼각수, 오각수, 육각수는 아래 식으로 구할 수 있습니다.
+  삼각수    Tn = n (n + 1) / 2     1, 3, 6, 10, 15, ... 
+  오각수    Pn = n (3n − 1) / 2     1, 5, 12, 22, 35, ... 
+  육각수    Hn = n (2n − 1)     1, 6, 15, 28, 45, ... 
+여기서  T285 = P165 = H143 =  40755 가 됩니다.
+오각수와 육각수도 되는, 그 다음으로 큰 삼각수를 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>46</t>
+    </r>
+  </si>
+  <si>
+    <t>(소수 + 2×제곱수)로 나타내지 못하는 가장 작은 홀수인 합성수는?</t>
+  </si>
+  <si>
+    <t>크리스티안 골드바흐는 모든 홀수인 합성수를 (소수 + 2×제곱수)로 나타낼 수 있다고 주장했습니다.
+  9 = 7 + 2×12
+  15 = 7 + 2×22
+  21 = 3 + 2×32
+  25 = 7 + 2×32
+  27 = 19 + 2×22
+  33 = 31 + 2×12 
+이 추측은 잘못되었음이 밝혀졌습니다.
+위와 같은 방법으로 나타낼 수 없는 가장 작은 홀수 합성수는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>47</t>
+    </r>
+  </si>
+  <si>
+    <t>서로 다른 네 개의 소인수를 갖는 수들이 처음으로 네 번 연속되는 경우는?</t>
+  </si>
+  <si>
+    <t>서로 다른 두 개의 소인수를 갖는 수들이 처음으로 두 번 연달아 나오는 경우는 다음과 같습니다.
+  14 = 2 × 7
+  15 = 3 × 5
+서로 다른 세 개의 소인수를 갖는 수들이 처음으로 세 번 연속되는 경우는 다음과 같습니다.
+  644 = 2² × 7 × 23
+  645 = 3 × 5 × 43
+  646 = 2 × 17 × 19
+서로 다른 네 개의 소인수를 갖는 수들이 처음으로 네 번 연속되는 경우를 찾으세요. 그 첫번째 숫자는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>48</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>1+ 22</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>+ 33+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t xml:space="preserve"> ... + 1000100</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>0의 마지막 10자리</t>
+    </r>
+  </si>
+  <si>
+    <t>1^1 + 2^2 + 3^3 + ... + 10^10 = 10405071317 입니다.
+1^1 + 2^2 + 3^3 + ... + 1000^1000 의 마지막 10자리 숫자는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>49</t>
+    </r>
+  </si>
+  <si>
+    <t>세 항이 소수이면서 다른 수의 순열이 되는 4자리 숫자의 등차수열 찾기</t>
+  </si>
+  <si>
+    <t>1487, 4817, 8147은 3330씩 늘어나는 등차수열입니다. 이 수열에는 특이한 점이 두 가지 있습니다.
+  •세 수는 모두 소수입니다.
+  •세 수는 각각 다른 수의 자릿수를 바꿔서 만들 수 있는 순열(permutation)입니다.
+1자리, 2자리, 3자리의 소수 중에서는 위와 같은 성질을 갖는 수열이 존재하지 않습니다. 하지만 4자리라면 위엣것 말고도 또 다른 수열이 존재합니다.
+그 수열의 세 항을 이었을 때 만들어지는 12자리 숫자는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>50</t>
+    </r>
+  </si>
+  <si>
+    <t>1백만 이하의 소수 중 가장 길게 연속되는 소수의 합으로 표현되는 수는?</t>
+  </si>
+  <si>
+    <t>41은 소수이면서 다음과 같은 6개의 연속된 소수의 합으로도 나타낼 수 있습니다.
+  41 = 2 + 3 + 5 + 7 + 11 + 13
+이것은 100 이하에서는 가장 길게 연속된 소수의 합으로 이루어진 소수입니다.
+1000 이하에서는 953이 연속된 소수 21개의 합으로 가장 깁니다.
+1백만 이하에서는 어떤 소수가 가장 길게 연속되는 소수의 합으로 표현될 수 있습니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+  </si>
+  <si>
+    <t>일부 숫자를 치환했을 때 8개의 서로 다른 소수가 생기는 가장 작은 소수</t>
+  </si>
+  <si>
+    <t>두 자리 숫자 *3의 첫번째 자리를 여러가지로 바꿨을 때 가능한 아홉 가지의 결과 중에서 13, 23, 43, 53, 73, 83의 여섯 개는 소수입니다.
+56**3 의 3번째와 4번째 자리를 동일한 숫자로 바꿔서 만들어지는 10개의 다섯자리 숫자 중에서는 아래에서 보듯이 7개가 소수가 되며, 이것은 이런 식으로 7개의 소수가 만들어지는 첫번째 경우입니다. 이 소수 집단의 첫번째 수인 56003은 이런 성질을 갖는 가장 작은 소수입니다.
+  56003, 56113, 56333, 56443, 56663, 56773, 56993
+위의 예처럼 원래의 일부를 동일한 숫자로 치환했을 때 8개의 소수 집단이 만들어지는 경우를 찾고, 그 집단에 속한 가장 작은 소수를 구하세요.
+치환하는 자리는 인접하지 않아도 되고, 가장 앞부분을 치환하는 경우 거기에 0은 올 수 없습니다.
+(역주: 번역이 잘못된 부분이 있어서 수정했습니다. 혼동을 드려서 죄송합니다. ^^; 2012.4.10)</t>
+  </si>
+  <si>
+    <r>
+      <t>52</t>
+    </r>
+  </si>
+  <si>
+    <t>2배, 3배, 4배, 5배, 6배의 결과도 같은 숫자로 이루어지는 가장 작은 수</t>
+  </si>
+  <si>
+    <t>125874를 2배 하면 251748이 되는데, 이 둘은 같은 숫자로 이루어져 있고 순서만 다릅니다.
+2배, 3배, 4배, 5배, 6배의 결과도 같은 숫자로 이루어지는 가장 작은 수는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>53</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1 ≤n≤ 100 일때nC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>r의</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t xml:space="preserve"> 값이 1백만을 넘는 경우는 모두 몇 번?</t>
+    </r>
+  </si>
+  <si>
+    <t>1,2,3,4,5 다섯 숫자 중에서 세 개를 고르는 것에는 다음과 같은 10가지 경우가 있습니다.
+  123, 124, 125, 134, 135, 145, 234, 235, 245, 345
+조합론이라는 분야에서는 이것을 5C3 = 10 이라고 표시하며, 일반적인 식은 아래와 같습니다.
+  nCr = (n! / r!(n−r)!' ) 단 r ≤ n 이고, n! = n×(n−1)×...×3×2×1 이며 0! = 1. 
+이 값은 n = 23 에 이르러서야 23C10 = 1144066 으로 처음 1백만을 넘게 됩니다.
+1 ≤ n ≤ 100 일때 nCr의 값이 1백만을 넘는 경우는 모두 몇 번입니까? (단, 중복된 값은 각각 계산합니다)</t>
+  </si>
+  <si>
+    <r>
+      <t>54</t>
+    </r>
+  </si>
+  <si>
+    <t>포커 게임에서 이긴 회수 구하기</t>
+  </si>
+  <si>
+    <t>포커라는 카드게임은 다섯 장으로 된 패의 높고 낮음에 따라 승부를 냅니다. (포커 규칙을 이미 아는 분이라면 규칙 설명 부분은 건너뛰셔도 좋습니다)
+카드 한 장은 아래와 같은 순서대로 값이 높아집니다.
+  2, 3, 4, 5, 6, 7, 8, 9, 10, J, Q, K, A
+다섯 장으로 이루어진 패의 계급(세칭 "족보")은, 낮은 것부터 높은 순서로 아래와 같습니다.
+  •High Card : 가장 높은 카드의 값으로 비교.
+  •One Pair : 한 쌍이 같은 카드.
+  •Two Pairs : 서로 다른 두 쌍이 같은 카드.
+  •Three of a Kind : 세 장이 같은 카드.
+  •Straight : 모든 카드가 연속된 숫자.
+  •Flush : 모든 카드의 무늬가 같음.
+  •Full House : 세 장이 같고, 또 한 쌍이 같음 (Three of a Kind + One Pair).
+  •Four of a Kind : 네 장이 같은 카드.
+  •Straight Flush : 모든 카드가 연속된 숫자이면서 무늬도 같음.
+  •Royal Flush : 10, J, Q, K, A가 무늬도 같음.
+두 사람의 패가 같은 종류의 계급이라면, 계급을 구성하는 카드 중 높은 쪽을 쥔 사람이 이깁니다. 예를 들면 8 원페어는 5 원페어를 이깁니다. 
+계급을 이루는 카드 숫자까지 같으면 (예: 둘 다 Q 원페어), 다른 카드를 높은 순서대로 비교해서 승부를 정합니다.
+텍스트파일 poker.txt 에는 두 선수가 벌인 1,000회의 승부가 저장되어 있습니다. (우클릭해서 다운로드 받으세요)
+한 줄에는 10장의 카드가 공백으로 분리되어 들어있는데, 앞의 다섯 장은 1번 선수 것이고 뒤의 다섯 장은 2번 선수의 패입니다. 잘못되거나 중복된 데이터는 없으며, 무승부도 없습니다.
+카드 숫자는 2, 3, ... , 9, T, J, Q, K, A 로 (숫자 10은 T로 표시),
+무늬는 C (Club - ♣), D (Diamond - ♦), H (Heart - ♥), S (Spade - ♠) 로 표시되어 있습니다.
+예를 들면 3C 3D 3S 9S 9D 의 경우 3 풀하우스가 됩니다.
+이 데이터를 분석하고, 1번 선수가 이긴 횟수를 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>55</t>
+    </r>
+  </si>
+  <si>
+    <t>10000 미만의 라이크렐 수 (Lychrel number) 세기</t>
+  </si>
+  <si>
+    <t>47이란 숫자를 골라서 뒤집은 다음 다시 원래 수에 더하면, 47 + 74 = 121 과 같이 대칭수(palindrome)가 됩니다.
+물론 모든 숫자가 이토록 쉽게 대칭수를 만들어내지는 않습니다. 예를 들어 349의 경우,
+  349 + 943 = 1292
+  1292 + 2921 = 4213
+  4213 + 3124 = 7337
+위에서 보는 것처럼 3번의 반복과정을 거쳐야 대칭수가 됩니다.
+196과 같은 몇몇 숫자들은 이와 같은 과정을 아무리 반복해도 대칭수가 되지 않을 것이라고 추측되는데, 이런 수를 라이크렐 수 (Lychrel number) 라고 부릅니다. 아직 증명되지는 않았지만, 문제 풀이를 위해서 일단 라이크렐 수가 존재한다고 가정을 하겠습니다.
+또한 1만 이하의 숫자들은, 50번 미만의 반복으로 대칭수가 되든지 라이크렐 수이든지 둘 중 하나라고 합니다.
+1만을 넘어서면 10677에 이르렀을 때 비로소 53번의 반복으로 4668731596684224866951378664 라는 28자리의 대칭수가 만들어집니다.
+그러면 1만 이하에는 몇 개의 라이크렐 수가 존재합니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>56</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>b형태의 자연수에 대해 자릿수 합의 최대값 구하기</t>
+    </r>
+  </si>
+  <si>
+    <t>구골(googol)은 10^100을 일컫는 말로, 1 뒤에 0이 백 개나 붙는 어마어마한 수입니다.
+100^100은 1 뒤에 0이 2백 개가 붙으니 상상을 초월할만큼 크다 하겠습니다.
+하지만 이 숫자들이 얼마나 크건간에, 각 자릿수를 모두 합하면 둘 다 겨우 1밖에 되지 않습니다.
+a, b 〈 100 인 자연수 a^b 에 대해서, 자릿수의 합이 최대인 경우 그 값은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>57</t>
+    </r>
+  </si>
+  <si>
+    <t>제곱근 2의 연분수꼴 살펴보기</t>
+  </si>
+  <si>
+    <t>제곱근 2는 다음과 같은 연분수의 형태로 나타낼 수 있습니다.
+  √ 2  = 1 + 1/(2 + 1/(2 + 1/(2 + ... ))) = 1.414213...
+위 식을 처음부터 한 단계씩 확장해 보면 아래와 같습니다.
+  1 + 1/2 = 3/2 = 1.5
+  1 + 1/(2 + 1/2) = 7/5 = 1.4
+  1 + 1/(2 + 1/(2 + 1/2)) = 17/12 = 1.41666...
+  1 + 1/(2 + 1/(2 + 1/(2 + 1/2))) = 41/29 = 1.41379... 
+그 다음은 99/70, 239/169, 577/408 로 확장이 되다가, 여덟번째인 1393/985 에 이르면 처음으로 분자의 자릿수가 분모의 자릿수를 넘어섭니다.
+처음부터 1천번째 단계까지 확장하는 중에, 분자의 자릿수가 분모보다 많아지는 경우는 몇 번이나 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>58</t>
+    </r>
+  </si>
+  <si>
+    <t>나선모양 격자의 대각선상에 있는 소수의 비율 추적하기</t>
+  </si>
+  <si>
+    <t>숫자를 1부터 시작해서 하나씩 늘려가며 아래와 같이 시계반대방향으로 감아가면 한 변의 크기가 7인 정사각형 소용돌이가 만들어집니다.
+  37 36 35 34 33 32 31
+  38 17 16 15 14 13 30
+  39 18  5  4  3 12 29
+  40 19  6  1  2 11 28
+  41 20  7  8  9 10 27
+  42 21 22 23 24 25 26
+  43 44 45 46 47 48 49
+우하단 대각선쪽으로 홀수 제곱수(9, 25, 49)들이 늘어서 있는 것이 눈에 띕니다만, 더 흥미로운 사실은 양 대각선상에 놓인 13개의 숫자 중 8개가 소수라는 것입니다. 그 비율은 대략 8/13 ≈ 62% 정도가 됩니다.
+이런 식으로 계속 소용돌이를 만들어갈 때, 양 대각선상의 소수 비율이 처음으로 10% 미만이 되는 것은 언제입니까? 정사각형 한 변의 크기로 답하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>59</t>
+    </r>
+  </si>
+  <si>
+    <t>XOR 방식으로 암호화된 메시지 깨기</t>
+  </si>
+  <si>
+    <t>컴퓨터상의 모든 문자들은 유일한 코드값에 대응되는데, 보통 ASCII 표준이 널리 쓰입니다. 예를 들면 대문자 A는 65, 별표(*)는 42, 소문자 k는 107라는 값을 가집니다.
+현대적인 암호화 기법 중에, 텍스트 파일의 내용을 ASCII 코드로 바꾸고 각 바이트를 비밀키의 값으로 XOR 시키는 것이 있습니다. 이 방법의 장점은 암호화와 복호화에 동일한 키를 사용할 수 있다는 것입니다. 예를 들어 65 XOR 42 = 107 이고, 107 XOR 42 = 65 가 됩니다.
+암호문을 절대 깰 수 없도록 하려면, 암호화할 문장의 길이와 같은 무작위의 비밀키를 만들면 됩니다. 암호문과 비밀키는 따로따로 보관해둬야 하고, 그 반쪽짜리 정보 두 개를 함께 확보하지 않는 한 해독은 불가능합니다.
+하지만 이 방법은 대부분의 경우 실용적이지 못하므로, 원문보다 짧은 비밀키를 사용하게 됩니다. 이런 경우 비밀키는 전체 메시지에 대해서 반복적으로 돌아가며 적용됩니다. 이 때 키의 길이는 보안상 충분할 정도로 길어야 하지만 또한 쉽게 기억할 수 있을 정도로 짧아야 한다는 미묘한 균형이 요구됩니다.
+이번 문제를 위해서 준비된 암호화 키는 단 3개의 영어 소문자이고, cipher1.txt 파일에 암호화된 ASCII 코드값이 들어있습니다. 원래의 메시지는 평범한 영어 문장임을 힌트로 삼아서 암호문을 해독하고, 원문에 포함된 모든 ASCII 코드 값의 총합을 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>60</t>
+    </r>
+  </si>
+  <si>
+    <t>다섯 소수 중 어떤 두 개를 이어붙여도 소수가 되는 수 찾기</t>
+  </si>
+  <si>
+    <t>네 개의 소수 3, 7, 109, 673은 상당히 특이한 성질이 있습니다. 넷 중에 아무것이나 두 개를 골라서 어떤 쪽으로 이어붙이던지 그 결과도 소수가 됩니다. 예를 들어 7과 109를 고르면 7109와 1097 또한 소수입니다.
+3, 7, 109, 673는 이런 성질을 가진 네 소수 중에서 그 합이 792로 가장 작습니다, 
+다섯 소수 중에 어떤 두 개를 골라 이어붙여도 소수가 되는 수들을 찾아서, 그 합의 최소값을 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>61</t>
+    </r>
+  </si>
+  <si>
+    <t>순환적인 성질을 갖는 4자리 다각수 여섯 개의 합</t>
+  </si>
+  <si>
+    <t>삼각수, 사각수, 오각수 같은 다각수들은 아래의 공식으로 만들 수 있습니다.
+  삼각수 P3,n = n(n+1)/2     1, 3, 6, 10, 15, ... 
+  사각수 P4,n = n2             1, 4, 9, 16, 25, ... 
+  오각수 P5,n = n(3n−1)/2  1, 5, 12, 22, 35, ... 
+  육각수 P6,n = n(2n−1)     1, 6, 15, 28, 45, ... 
+  칠각수 P7,n = n(5n−3)/2  1, 7, 18, 34, 55, ... 
+  팔각수 P8,n = n(3n−2)     1, 8, 21, 40, 65, ... 
+그런데 4자리 숫자 8128, 2882, 8281 (순서대로) 에는 세 가지의 재미있는 성질이 있습니다.
+  1.각 숫자들은 서로 꼬리를 물고 순환됩니다. 각 숫자의 뒤쪽 두 자리는 다음 숫자의 앞쪽 두 자리가 되는 식입니다.
+  2.각 숫자는 서로 다른 다각수인데, 여기서는 삼각수 (P3,127=8128), 사각수 (P4,91=8281), 오각수 (P5,44=2882)가 대응됩니다.
+  3.이런 성질을 갖는 4자리의 숫자 세 개는 이 숫자들이 유일합니다.
+위와 같이 순환되면서 서로 다른 다각수(삼각수 ~ 팔각수)이기도 한 4자리 숫자 여섯 개의 유일한 순서쌍을 찾고, 그 합을 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>62</t>
+    </r>
+  </si>
+  <si>
+    <t>자릿수로 만든 순열 중에서 5개가 세제곱수인 가장 작은 숫자는?</t>
+  </si>
+  <si>
+    <t>세제곱수인 41063625 (=345^3) 로 순열을 만들어보면, 그 중에서 56623104 (=384^3)와 66430125 (=405^3)가 또 세제곱수입니다.
+실제 41063625은, 자릿수로 만든 순열 중에서 3개가 세제곱수인 가장 작은 수입니다.
+그러면 자릿수로 만든 순열 중에서 5개가 세제곱수인 가장 작은 숫자는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>63</t>
+    </r>
+  </si>
+  <si>
+    <t>n자리 숫자이면서n제곱수도 되는 양의 정수는 모두 몇 개?</t>
+  </si>
+  <si>
+    <t>다섯 자리 숫자인 16807은 7^5으로 5제곱수입니다. 또, 아홉 자리 숫자인 134217728은 8^9으로 9제곱수입니다.
+n자리 숫자이면서 n제곱수도 되는 양의 정수는 모두 몇 개나 있습니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>64</t>
+    </r>
+  </si>
+  <si>
+    <t>제곱근을 연분수로 나타낼 때 반복 주기가 홀수인 경우 세기</t>
+  </si>
+  <si>
+    <r>
+      <t>65</t>
+    </r>
+  </si>
+  <si>
+    <t>e의 100번째 연분수 확장 값의 분자 자릿수를 모두 더하면?</t>
+  </si>
+  <si>
+    <r>
+      <t>66</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>2– Dy2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>= 1 형태의 디오판토스 방정식 풀기</t>
+    </r>
+  </si>
+  <si>
+    <t>다음과 같은 2차 디오판토스 방정식이 있습니다.
+  x2 – Dy2 = 1
+(역주: 디오판토스 방정식은 정수해만 허용하는 부정다항방정식입니다. 그 중에서도 여기 나온 형태는 펠의 방정식이라고 하는데, x/y로 √D의 근사값을 구하는 데 이용됩니다.)
+예를 들어서 D=13일 때 x를 최소화하는 해는 6492 – 13×1802 = 1 이 됩니다.
+D가 제곱수일 경우에는 위 식을 만족하는 자연수 해는 없다고 볼 수 있습니다.
+D = {2, 3, 5, 6, 7} 에 대해서 x를 최소화하는 자연수 해를 찾아보면, 아래와 같은 결과를 얻게 됩니다.
+  3^2 – 2×2^2 = 1
+  2^2 – 3×1^2 = 1
+  9^2 – 5×4^2 = 1
+  5^2 – 6×2^2 = 1
+  8^2 – 7×3^2 = 1
+위에서 보듯이 D ≤ 7 인 경우에 대해 x를 최소화하는 해를 구하면, x의 값이 가장 큰 것은 D=5일 때입니다.
+D ≤ 1000 인 경우에 대해 x를 최소화하는 해를 구하면, 가장 큰 x의 값을 갖는 D는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>67</t>
+    </r>
+  </si>
+  <si>
+    <t>삼각형에서 경로의 합 중 최대값을 구하는 효율적인 방법은?</t>
+  </si>
+  <si>
+    <t>아래와 같은 삼각형의 꼭대기에서 인접한 숫자를 따라 내려가는 경로의 합을 계산해보면, 붉은 색으로 표시한 경우가 3 + 7 + 4 + 9 = 23으로 가장 큽니다.
+     3
+    7 4
+   2 4 6
+  8 5 9 3
+텍스트 파일 triangle.txt (우클릭해서 다운로드)에는 100줄짜리 삼각형 숫자 데이터가 들어 있습니다. 꼭대기에서 바닥에 이르는 경로의 합 중 최대값은 얼마입니까?
+참고: 이 문제는 18번 문제와 비슷하지만 훨씬 더 어려운 버전입니다. 이 문제를 풀려고 모든 경로를 계산하는 것은 가능하지 않은데, 경우의 수가 모두 299 이나 되기 때문입니다. 일 초에 1조 (1012)개의 경로를 계산할 수 있다고 해도, 모든 경우의 수를 계산하려면 200억년이 걸립니다. 이 문제를 해결할 수 있는 효율적인 알고리즘을 찾아보시기 바랍니다.</t>
+  </si>
+  <si>
+    <r>
+      <t>68</t>
+    </r>
+  </si>
+  <si>
+    <t>마방진 성질을 갖는 5각 도형에서 얻을 수 있는 16자리 수의 최대값 구하기</t>
+  </si>
+  <si>
+    <r>
+      <t>69</t>
+    </r>
+  </si>
+  <si>
+    <t>n/φ(n)이 최대가 되는 1백만 이하의n찾기</t>
+  </si>
+  <si>
+    <t>오일러의 피(phi)함수 φ(n)은 n보다 작거나 같으면서 n과 서로 소인 숫자의 개수를 나타냅니다. 예를 들어, 9보다 작거나 같으면서 9와 서로 소인 것은 1, 2, 4, 5, 7, 8이므로 φ(9)=6이 됩니다.
+   n | 서로 소인 수  | φ(n) | n/φ(n)
+   2 | 1                 |   1   |   2 
+   3 | 1, 2              |   2   |  1.5 
+   4 | 1, 3              |   2   |   2 
+   5 | 1, 2, 3, 4        |   4   |  1.25 
+   6 | 1, 5               |   2   |   3 
+   7 | 1, 2, 3, 4, 5, 6  |   6   | 1.1666... 
+   8 | 1, 3, 5, 7        |   4   |    2 
+   9 | 1, 2, 4, 5, 7, 8  |   6   |  1.5 
+  10 | 1, 3, 7, 9        |   4   |  2.5 
+위에서 보듯이 n ≤ 10인 경우 n/φ(n)의 값은 n=6일때 최대가 됩니다.
+n이 1,000,000 이하의 자연수일 때, n/φ(n)는 언제 최대가 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>70</t>
+    </r>
+  </si>
+  <si>
+    <t>φ(n)이n의 순열이 되는 수 조사하기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">오일러 피(phi) 함수 φ(n)은 n보다 작거나 같은 자연수 중 n과 서로 소인 숫자의 개수를 나타냅니다. 예를 들어 9 이하에서 9와 서로 소인 자연수는 1, 2, 4, 5, 7, 8이므로 φ(9)=6입니다.
+또, 1은 어떤 자연수와도 서로 소이므로 φ(1)=1입니다.
+φ(87109)의 값은 79180인데, 흥미롭게도 79180은 87109로 만들 수 있는 순열 중 하나입니다.
+1 &lt; n &lt; 107 이고 φ(n)이 n의 순열이 되는 수 중에서, n/φ(n)이 최소인 n은 얼마입니까? </t>
+  </si>
+  <si>
+    <r>
+      <t>71</t>
+    </r>
+  </si>
+  <si>
+    <t>기약 진분수를 커지는 순으로 늘어놓기</t>
+  </si>
+  <si>
+    <t>n과 d가 양의 정수이고 n&lt;d인 분수 n/d을 GCD(n, d) = 1일 때 기약 진분수라고 부르기로 합니다.
+d ≤ 8 인 기약 진분수들을 커지는 순으로 늘어놓으면 아래와 같습니다.
+  1/8, 1/7, 1/6, 1/5, 1/4, 2/7, 1/3, 3/8, 2/5, 3/7, 1/2, 4/7, 3/5, 5/8, 2/3, 5/7, 3/4, 4/5, 5/6, 6/7, 7/8
+위에서 보듯이 3/7의 바로 앞에는 2/5가 오게 됩니다.
+d ≤ 1,000,000 인 기약 진분수들을 커지는 순으로 늘어놓았을 때, 3/7 바로 앞에 오는 수의 분자는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>72</t>
+    </r>
+  </si>
+  <si>
+    <t>분모가 1백만 이하인 기약 진분수의 개수</t>
+  </si>
+  <si>
+    <t>n과 d가 양의 정수이고 n&lt;d인 분수 n/d을 GCD(n, d) = 1일 때 기약 진분수라고 부르기로 합니다.
+d ≤ 8 인 기약 진분수들을 커지는 순으로 늘어놓으면 아래와 같고, 개수는 모두 21개입니다.
+  1/8, 1/7, 1/6, 1/5, 1/4, 2/7, 1/3, 3/8, 2/5, 3/7, 1/2, 4/7, 3/5, 5/8, 2/3, 5/7, 3/4, 4/5, 5/6, 6/7, 7/8
+d ≤ 1,000,000 인 경우, 기약 진분수는 모두 몇 개나 있습니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>73</t>
+    </r>
+  </si>
+  <si>
+    <t>분모가 12,000 이하일 때 1/3과 1/2 사이에 위치한 기약 진분수의 개수</t>
+  </si>
+  <si>
+    <t>n과 d가 양의 정수이고 n&lt;d인 분수 n/d을 GCD(n, d) = 1일 때 기약 진분수라고 부르기로 합니다.
+d ≤ 8 인 기약 진분수들을 커지는 순으로 늘어놓으면 아래와 같습니다.
+  1/8, 1/7, 1/6, 1/5, 1/4, 2/7, 1/3, 3/8, 2/5, 3/7, 1/2, 4/7, 3/5, 5/8, 2/3, 5/7, 3/4, 4/5, 5/6, 6/7, 7/8
+위에서 보듯이, 1/3과 1/2 사이에는 기약 진분수가 세 개 있습니다.
+그러면 d ≤ 12,000일 때 1/3과 1/2 사이의 기약 진분수는 몇 개나 있습니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>74</t>
+    </r>
+  </si>
+  <si>
+    <t>자릿수의 계승값을 더해갈 때, 반복이 일어나기 전의 단계가 60번인 경우 찾기</t>
+  </si>
+  <si>
+    <t>145는 각 자릿수의 계승값을 모두 더했을 때 자기 자신이 되는 수로 잘 알려져 있습니다.
+  1! + 4! + 5! = 1 + 24 + 120 = 145
+그보다 덜 유명하긴 하지만 169는 위와 같은 방법으로 계산해서 자기 자신으로 되돌아오는 데 가장 많은 단계를 거치는 숫자로, 그런 특성을 가진 숫자는 3개밖에 없다고 합니다.
+  169 → 363601 → 1454 → 169
+  871 → 45361 → 871
+  872 → 45362 → 872
+어떤 숫자로 시작해도 결국 위와 같은 반복 루프에 들어간다는 사실은 어렵지 않게 증명이 가능한데, 몇 개 숫자의 예를 들면 다음과 같습니다.
+  69 → 363600 → 1454 → 169 → 363601 (→ 1454)
+  78 → 45360 → 871 → 45361 (→ 871)
+  540 → 145 (→ 145)
+69로 시작하면, 반복이 일어나기 전에 다섯 번의 단계를 거친 다음에 루프에 들어갑니다. 1백만 이하의 숫자로 시작하는 경우는 최대 60번의 반복되지 않는 단계가 존재합니다.
+1백만 이하의 숫자로 시작했을 때, 반복되지 않는 단계를 정확히 60번 거치는 경우는 모두 몇 번이나 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>75</t>
+    </r>
+  </si>
+  <si>
+    <t>직각삼각형을 만들어내는 방법이 한 가지 뿐인 경우 세기</t>
+  </si>
+  <si>
+    <t>긴 철사를 구부려서 세 변이 정수인 직각삼각형을 만들 때, 그 방법이 한 가지 뿐인 경우는 12cm를 최소로 해서 아래와 같이 여러 개가 있습니다.
+  12 cm: (3,4,5)
+  24 cm: (6,8,10)
+  30 cm: (5,12,13)
+  36 cm: (9,12,15)
+  40 cm: (8,15,17)
+  48 cm: (12,16,20) 
+반면에 20cm의 경우처럼 세 변이 정수인 직각삼각형을 만들 수 없을 때도 있고, 여러 종류의 직각삼각형을 만들 수 있을 때도 있습니다. 예를 들어 120cm의 철사로는 세 가지의 서로 다른 직각삼각형이 만들어집니다.
+  120 cm: (30,40,50), (20,48,52), (24,45,51)
+그러면 길이가 1,500,000 이하인 철사를 가지고 세 변이 정수인 직각삼각형을 만들 때, 그 길이로는 한 가지 방법으로만 만들 수 있게 되는 경우는 모두 얼마나 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>76</t>
+    </r>
+  </si>
+  <si>
+    <t>숫자 100을 두 개 이상의 자연수의 합으로 나타내는 방법은 모두 몇 가지?</t>
+  </si>
+  <si>
+    <t>숫자 5를 자연수의 합으로 나타내는 데는 모두 여섯 가지 방법이 있습니다.
+  4 + 1
+  3 + 2
+  3 + 1 + 1
+  2 + 2 + 1
+  2 + 1 + 1 + 1
+  1 + 1 + 1 + 1 + 1 
+그러면 숫자 100을 두 개 이상의 자연수의 합으로 나타내는 방법은 모두 몇 가지나 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>77</t>
+    </r>
+  </si>
+  <si>
+    <t>소수의 합으로 나타내는 방법이 5000가지가 넘는 최초의 숫자는?</t>
+  </si>
+  <si>
+    <t>숫자 10을 소수의 합으로 나타내는 방법은 모두 다섯 가지가 있습니다.
+  7 + 3
+  5 + 5
+  5 + 3 + 2
+  3 + 3 + 2 + 2
+  2 + 2 + 2 + 2 + 2 
+소수의 합으로 나타내는 방법이 5000가지가 넘는 최초의 숫자는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>78</t>
+    </r>
+  </si>
+  <si>
+    <t>동전을 여러 더미로 나누는 경우의 수 세기</t>
+  </si>
+  <si>
+    <t>n개의 동전을 여러 더미로 나누는 경우의 수를 p(n)이라고 나타내기로 합니다.
+예를 들어 동전 다섯 개는 아래와 같이 일곱 가지 방법으로 나눌 수 있으므로 p(5) = 7이 됩니다.
+  OOOOO 
+  OOOO   O 
+  OOO   OO 
+  OOO   O   O 
+  OO   OO   O 
+  OO   O   O   O 
+  O   O   O   O   O 
+p(n)이 1백만으로 나누어 떨어지는 가장 작은 n의 값은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>79</t>
+    </r>
+  </si>
+  <si>
+    <t>접속 기록으로부터 비밀번호 알아내기</t>
+  </si>
+  <si>
+    <t>온라인 뱅킹에서 흔히 쓰이는 보안 기법 중에는, 비밀번호에 포함된 숫자를 랜덤하게 세 개 입력하도록 하는 것이 있습니다. 
+예를 들어 531278이라는 비밀번호에 대해서 2번째, 3번째, 5번째 숫자를 입력하도록 하는 식입니다. 이 때 올바른 입력은 317이 됩니다.
+첨부한 텍스트 파일 keylog.txt에는 로그인에 성공한 어떤 사용자의 입력 기록이 50건 담겨져 있습니다. (비밀번호의 길이는 알 수 없습니다)
+3개의 숫자는 항상 앞쪽부터 순서대로 요청된다고 할 때, 위의 접속 기록에서 알아낼 수 있는 가장 짧은 길이의 비밀번호는 무엇입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>80</t>
+    </r>
+  </si>
+  <si>
+    <t>무리수인 제곱근들의 자릿수 더하기</t>
+  </si>
+  <si>
+    <t>자연수의 제곱근이 정수가 아니라면 무리수가 되고, 이런 경우 소수점 밑으로 반복되는 패턴이 전혀 없는 숫자들이 무한히 전개됩니다.
+2의 제곱근은 1.41421356237309504880... 인데, 처음 100개까지의 자릿수를 모두 더하면 475입니다.
+1부터 100까지의 자연수 중에서 제곱근이 무리수인 경우에 대해, 처음 100개까지의 자릿수를 더한 값들의 총합은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>81</t>
+    </r>
+  </si>
+  <si>
+    <t>오른쪽과 아래로만 움직이면서 좌상단→우하단으로 가는 경로의 합이 최소인 경우는?</t>
+  </si>
+  <si>
+    <t>아래와 같은 5×5 행렬이 있습니다. 좌측 상단에서 출발하고 오른쪽이나 아래로만 움직이면서 우측 하단까지 가는 경로의 합을 구해 보면, 빨갛게 표시된 경로가 2427로서 가장 작습니다.
+  131 673 234 103 18 
+  201 96 342 965 150 
+  630 803 746 422 111 
+  537 699 497 121 956 
+  805 732 524 37 331
+31KB짜리 파일 matrix.txt에는 80×80 행렬의 정보가 들어있습니다. 위와 같은 방법으로 이 행렬의 좌측 상단에서 출발하여 우측 하단까지 갈 때, 경로 합의 최소값은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>82</t>
+    </r>
+  </si>
+  <si>
+    <t>맨 왼쪽 열에서 맨 오른쪽 열까지 가는 경로의 합이 최소인 경우는?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(참고: 이 문제는 81번 문제의 좀 더 어려운 버전입니다)
+아래와 같은 5×5 행렬이 있습니다. 맨 왼쪽 열의 아무 곳에서나 출발하여 위/아래/오른쪽으로만 움직이면서 맨 오른쪽 열까지 갈 때, 빨갛게 표시된 경로의 합이 994로 가장 작습니다.
+  131 673 234 103 18 
+  201 96 342 965 150 
+  630 803 746 422 111 
+  537 699 497 121 956 
+  805 732 524 37 331 
+31KB짜리 파일 matrix.txt에는 80×80 행렬의 정보가 들어있습니다. 위와 같은 방법으로 이 행렬의 맨 왼쪽 열에서 출발하여 맨 오른쪽 열까지 갈 때, 경로 합의 최소값은 얼마입니까? </t>
+  </si>
+  <si>
+    <r>
+      <t>83</t>
+    </r>
+  </si>
+  <si>
+    <t>상하좌우로 움직여서 좌상단→우하단으로 가는 경로의 합이 최소인 경우는?</t>
+  </si>
+  <si>
+    <t>(참고: 이 문제는 81번 문제의 훨씬 더 어려운 버전입니다) 
+아래와 같은 5×5 행렬이 있습니다. 좌측 상단에서 출발해서 상하좌우로 움직이면서 우측 하단까지 가는 경로의 합을 구해 보면, 빨갛게 표시된 경로가 2297로서 가장 작습니다.
+  131 673 234 103 18 
+  201 96 342 965 150 
+  630 803 746 422 111 
+  537 699 497 121 956 
+  805 732 524 37 331 
+31KB짜리 파일 matrix.txt에는 80×80 행렬의 정보가 들어있습니다. 위와 같은 방법으로 이 행렬의 좌측 상단에서 출발하여 우측 하단까지 갈 때, 경로 합의 최소값은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>84</t>
+    </r>
+  </si>
+  <si>
+    <t>모노폴리 게임을 4면체 주사위로 할 때 가장 많이 방문하는 칸은?</t>
+  </si>
+  <si>
+    <r>
+      <t>85</t>
+    </r>
+  </si>
+  <si>
+    <t>사각 격자 안에 포함된 사각형 개수 세기</t>
+  </si>
+  <si>
+    <t>3×2 크기의 격자를 주의 깊게 조사해보면, 그 안에는 아래 그림과 같이 18개의 사각형이 포함됨을 알 수 있습니다. 
+  ■□□　■■□　■■■
+  □□□　□□□　□□□
+  　6　　　　4　　　　2
+  ■□□　■■□　■■■
+  ■□□　■■□　■■■
+  　3　　　　2　　　　1
+이런 식으로 세었을 때 사각형을 정확히 2백만개 포함하는 격자는 존재하지 않는다고 합니다. 2백만에 가장 근접한 개수의 사각형을 포함하는 격자를 찾고, 그 넓이를 구해보세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>86</t>
+    </r>
+  </si>
+  <si>
+    <t>육면체의 한쪽 구석에서 다른 구석으로 가는 최단 경로 찾기</t>
+  </si>
+  <si>
+    <t>크기가 6×5×3인 직육면체 모양의 방 안 한쪽 구석에 거미(S)가 앉아 있고, 반대쪽 구석에는 파리(F)가 앉아 있습니다. 거미가 방의 표면을 가로질러서 파리에게 가는 가장 짧은 "직선" 경로의 거리는 아래 그림과 같이 10 이 됩니다.
+하지만 일반적인 경우 가장 짧은 경로는 많게는 3개까지 있을 수 있고, 경로의 길이가 정수값이 아닐 수도 있습니다.
+각 변의 길이가 모두 정수이고 최대 크기가 M×M×M 인 모든 직육면체에 대해서 최단 경로가 정수인 경우를 조사했을 때, M=100 이면 모두 2060가지가 있고 이것은 경우의 수가 2000이 넘는 최소의 M 값입니다 (M=99일 때는 1975).
+그러면 이런 조건을 만족하는 직육면체의 수가 1백만을 넘는 최소의 M은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>87</t>
+    </r>
+  </si>
+  <si>
+    <t>소수의 제곱 + 소수의 3제곱 + 소수의 4제곱으로 나타낼 수 있는 숫자</t>
+  </si>
+  <si>
+    <t>(소수의 제곱 + 소수의 3제곱 + 소수의 4제곱)으로 나타낼 수 있는 가장 작은 수는 28입니다.
+50 미만의 숫자 중에서 이런 수는 모두 네 개가 있습니다.
+  28 = 2^2 + 2^3 + 2^4
+  33 = 3^2 + 2^3 + 2^4
+  49 = 5^2 + 2^3 + 2^4
+  47 = 2^2 + 3^3 + 2^4
+5천만 미만의 수 중에서 이렇게 나타낼 수 있는 숫자는 모두 몇 개나 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>88</t>
+    </r>
+  </si>
+  <si>
+    <t>일정한 개수의 숫자들을 더해도 곱해도 같은 값이 되는 경우 조사하기</t>
+  </si>
+  <si>
+    <t>두 개 이상의 자연수 { a1, a2, ... , ak } 를 모두 더한 값도 N이고 곱한 값도 N이 될 때, 즉 N = a1 + a2 + ... + ak = a1 × a2 × ... × ak 이면 자연수 N을 product-sum number라고 부르기로 합니다. 
+예를 들면 6 = 1+2+3 = 1×2×3 같은 경우입니다.
+이제 k개의 숫자에 대해서 이런 성질을 만족하는 최소의 N 값을 구해보면, k = 2, 3, 4, 5, 6일 때 다음과 같은 결과를 얻습니다.
+  k=2 : 4 = 2×2 = 2+2
+  k=3 : 6 = 1×2×3 = 1+2+3
+  k=4 : 8 = 1×1×2×4 = 1+1+2+4
+  k=5 : 8 = 1×1×2×2×2 = 1+1+2+2+2
+  k=6 : 12 = 1×1×1×1×2×6 = 1+1+1+1+2+6
+위에서 보듯이 2 ≤ k ≤ 6 의 범위에서 최소의 product-sum number들을 모두 더하면 4+6+8+12 = 30 이 됨을 알 수 있습니다 (중복 제외). 
+동일하게 2 ≤ k ≤ 12 범위에서 최소 product-sum number들을 구하면 {4, 6, 8, 12, 15, 16}이고, 모두 더하면 61입니다.
+그러면 2 ≤ k ≤ 12000 의 범위에 대해 최소 product-sum number들을 구했을 때 그 합은 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>89</t>
+    </r>
+  </si>
+  <si>
+    <t>로마숫자 최적화하기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I = 1
+  V = 5
+  X = 10
+  L = 50
+  C = 100
+  D = 500
+  M = 1000
+뺄셈에 대한 몇 가지 규칙
+  i. 뺄셈을 구성하는 부분은 I, X, C로만 시작할 수 있다. 
+  ii.I는 V, X 앞에만 올 수 있다. 
+  iii.X는 L, C 앞에만 올 수 있다. 
+  iv.C는 D, M 앞에만 올 수 있다 
+11KB 크기의 텍스트 파일 roman.txt에는 표기법상으로 올바르지만 꼭 최적화되었다는 보장은 없는 1만개의 로마숫자가 들어있습니다. 각 숫자의 문자들은 물론 작아지는 순으로 배열되어 있으며, (위 상자글에 언급된) 뺄셈을 위한 4가지 규칙을 준수합니다.
+숫자들을 최적화된 형태로 모두 고쳐썼을 때, 줄어든 문자 수는 모두 몇 개나 됩니까?
+참고 : 이 파일에 들어있는 모든 로마숫자에서 동일한 문자가 4개를 넘는 경우는 없습니다.</t>
+  </si>
+  <si>
+    <r>
+      <t>90</t>
+    </r>
+  </si>
+  <si>
+    <t>정육면체 두 개로 제곱수 만들기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">정육면체 두 개의 각 면에 0부터 9까지 중에서 서로 다른 숫자를 써서 나란히 세우면 여러 가지의 2자리 숫자를 만들 수 있습니다. 예를 들어 제곱수인 64를 만들려면 아래와 같이 하면 됩니다. 
+  6 | 4
+양쪽에 배정할 숫자들을 주의깊게 고르면, 이런 방식으로 100 미만의 모든 제곱수 (01, 04, 09, 16, 25, 36, 49, 64, 81)를 나타내는 것이 가능합니다. 
+그렇게 하는 방법 하나는, 한 쪽에 {0, 5, 6, 7, 8, 9}를 쓰고 다른 쪽에 {1, 2, 3, 4, 8, 9}를 쓰는 것입니다. 
+하지만 6과 9는 뒤집었을 때 같은 모양이 되므로, 숫자를 만들 때 뒤집는 것을 허용하기로 합니다. 이렇게 해서 {0, 5, 6, 7, 8, 9}와 {1, 2, 3, 4, 6, 7}의 조합으로도 아홉 개의 모든 제곱수를 나타낼 수가 있습니다. 만약 그렇지 않다면 이 조합에서는 09를 표시할 방법이 없게 됩니다. 
+숫자의 조합을 정할 때 순서는 상관하지 않기로 합니다. 따라서 {1, 2, 3, 4, 5, 6} 은 {3, 6, 4, 1, 2, 5} 와 같은 조합을 나타냅니다.
+원칙대로 하자면 {1, 2, 3, 4, 5, 6} 은 {1, 2, 3, 4, 5, 9}과 다른 조합이지만, 6과 9를 뒤집을 수 있게 허용하면 둘 다 동일하게 {1, 2, 3, 4, 5, 6, 9}라는 확장된 숫자 조합을 나타내게 됩니다.
+이렇게 했을 때, 100 미만의 제곱수를 모두 나타낼 수 있는 숫자의 조합은 모두 몇 가지나 됩니까? </t>
+  </si>
+  <si>
+    <r>
+      <t>91</t>
+    </r>
+  </si>
+  <si>
+    <t>사분면 안의 직각삼각형 개수 세기</t>
+  </si>
+  <si>
+    <t>정수 좌표계 상에서 두 점 P (x1, y1) 와 Q (x2, y2) 를 잡고 원점 O(0,0)와 이으면 삼각형 ΔOPQ가 만들어집니다. 
+x, y 좌표값이 0과 2 사이일 때, 즉 0 ≤ x1, y1, x2, y2 ≤ 2 일 때 만들 수 있는 삼각형 중에서 직각삼각형은 모두 14개입니다. 
+0 ≤ x1, y1, x2, y2 ≤ 50 일 때는 직각삼각형이 모두 몇 개나 만들어질까요?</t>
+  </si>
+  <si>
+    <r>
+      <t>92</t>
+    </r>
+  </si>
+  <si>
+    <t>자릿수를 제곱해서 더해가는 수열의 신기한 성질</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어떤 수의 각 자릿수를 제곱해서 모두 더하고, 전에 나왔던 숫자가 다시 나올때까지 같은 과정을 거듭합니다. 그러면 아래의 예와 같은 일련의 숫자들을 얻습니다.
+  44 → 32 → 13 → 10 → 1 → 1
+  85 → 89 → 145 → 42 → 20 → 4 → 16 → 37 → 58 → 89
+위에서 알 수 있듯이 일단 1 또는 89에 도달하면 그 다음부터는 정해진 숫자들을 무한히 반복하게 됩니다. 정말 신기한 것은 어떤 숫자로 시작해도 결국에는 1이나 89에 도달한다는 사실입니다.
+그러면 1천만 미만의 자연수 중에서, 이런 과정을 거쳐 89에 도달하는 수는 몇 개나 있습니까? </t>
+  </si>
+  <si>
+    <r>
+      <t>93</t>
+    </r>
+  </si>
+  <si>
+    <t>숫자 4개와 사칙연산을 써서 가장 길게 이어지는 숫자 만들기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1부터 4까지의 숫자를 한 번씩만 쓰면서, 사칙연산 기호(+, −, *, /)와 괄호를 적절히 조합하면 각기 다른 양의 정수를 여럿 만들어낼 수 있습니다. 
+몇 가지 예를 들자면 아래와 같습니다.
+  8 = (4 * (1 + 3)) / 2
+  14 = 4 * (3 + 1 / 2)
+  19 = 4 * (2 + 3) − 1
+  36 = 3 * 4 * (2 + 1)
+이 때 12 + 34 처럼 숫자들을 이어붙이지는 않기로 합니다. 
+이렇게 해서 1 ~ 4의 숫자로는 31개의 다른 결과값(최대 36)을 만들 수 있고, 결과값 중 1부터 28까지는 중간에 끊김 없이 계속 이어집니다. 
+a &lt; b &lt; c &lt; d 인 숫자 네 개로 위와 같이 했을 때 결과값이 1부터 가장 길게 이어지는 숫자들을 찾고, abcd 의 형태로 답을 제시하세요. </t>
+  </si>
+  <si>
+    <r>
+      <t>94</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>정수 둘레와 정수 넓이를 갖는거</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>의 정삼각형찾</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>기</t>
+    </r>
+  </si>
+  <si>
+    <t>정삼각형에서 각 변의 길이가 정수이면 그 넓이는 정수가 아님을 쉽게 증명할 수 있습니다. 하지만, 거의 정삼각형에 가깝다고 볼 수 있는 5-5-6의 둘레를 가진 삼각형은 넓이가 12로서 정수값이 됩니다. 
+이제 이등변삼각형에서 등변인 한 변과 등변 아닌 변의 길이 차이가 1 이하인 경우에 대해서만 거의 정삼각형이라는 표현을 쓰기로 합니다. 그러면, 둘레의 길이가 10억을 넘지 않으면서 변의 길이도 정수이고 넓이도 정수인 거의 정삼각형들을 찾아서 그 둘레를 전부 더하면 얼마가 됩니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>95</t>
+    </r>
+  </si>
+  <si>
+    <t>1백만 이하의 숫자로 이루어진 친화고리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어떤 수에 대해서 자신을 제외한 약수들을 진약수라 부르기로 합니다. 예를 들어 28의 진약수는 1, 2, 4, 7, 14입니다. 이것을 모두 더하면 다시 28이 되는데, 이런 수들을 완전수라고 부릅니다. 
+흥미롭게도 220의 진약수를 모두 더하면 284이고, 284의 진약수의 합은 다시 220이 됩니다. 이런 경우를 친화쌍(또는 우애수)이라고 합니다. 
+상대적으로 덜 알려졌지만, 비슷한 성질을 갖는 일련의 수들이 연쇄적으로 늘어서는 경우도 있습니다. 예를 들어 12496에서 시작하면 아래와 같은 다섯 개의 숫자로 이루어지는 수열을 얻게 됩니다.
+  12496 → 14288 → 15472 → 14536 → 14264 (→ 12496 → ...)
+이 수열은 다시 처음 숫자로 돌아가므로, "친화고리"라고 부를 수 있겠습니다. 
+1백만 이하의 숫자로만 이루어진 친화고리 중에서 길이가 가장 긴 고리를 찾아보세요. 그 수열을 이루는 숫자 중 가장 작은 것은 얼마입니까? </t>
+  </si>
+  <si>
+    <r>
+      <t>96</t>
+    </r>
+  </si>
+  <si>
+    <t>스도쿠 퍼즐 풀기</t>
+  </si>
+  <si>
+    <t>스도쿠(일본어로 '숫자 자리'라는 뜻)는 인기있는 숫자 퍼즐입니다. 그 유래는 확실치 않지만, 비슷하면서 훨씬 더 어려운 라틴 방진(Latin Squares)이라는 퍼즐을 고안했던 레온하르트 오일러의 영향을 받았음이 분명합니다. 스도쿠는 가로 9칸, 세로 9칸으로 이루어진 표에서 각 행과 열, 그리고 작은 3x3 격자 안에 모두 1부터 9까지의 숫자가 한번씩만 들어가도록 빈 칸을 채우는 것이 목적입니다.
+잘 만들어진 스도쿠 퍼즐은 유일한 해답을 가지며 논리적인 방법으로 해결이 가능하지만, 가끔은 선택의 경우를 줄이기 위해 "찍고 맞춰보는" 과정이 필요할 수도 있습니다 (여기에 대해서는 논란이 많습니다). 퍼즐의 난이도는 이러한 탐색과정의 복잡도에 따라 결정됩니다. 위에 나온 예제는 직접적인 추론에 의해 해결이 가능해서 쉬운 편에 속합니다. 
+6KB의 텍스트 파일 sudoku.txt에는 다양한 난이도의 스도쿠 퍼즐이 50개 들어 있습니다. 모든 문제의 해답은 유일합니다 (위에 나온 예제가 첫번째 문제입니다). 
+50개의 퍼즐을 모두 푼 다음에, 각 해답지에서 맨 왼쪽 위의 숫자 3개를 이어붙인 수를 모두 더하면 얼마가 됩니까? (위 예제의 경우 483과 같은 수를 말합니다)</t>
+  </si>
+  <si>
+    <r>
+      <t>97</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>메르센 수가 아닌 소수 28433×2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+      </rPr>
+      <t>7830457+1의 마지막 10자리는?</t>
+    </r>
+  </si>
+  <si>
+    <t>자릿수가 백만이 넘는 소수는 1999년에 처음 발견되었고, 이 수는 2^6972593−1 모양의 메르센 소수로 2,098,960자리입니다. 그 후로 2^p−1 형태의 더 큰 메르센 소수들이 뒤를 이었습니다. 
+하지만 2004년, 메르센 소수가 아닌 2,357,207자리의 어마어마한 소수가 발견되었는데, 그 수는 바로 28433×2^7830457+1 입니다. 
+이 소수의 마지막 10자리는 얼마입니까?</t>
+  </si>
+  <si>
+    <r>
+      <t>98</t>
+    </r>
+  </si>
+  <si>
+    <t>제곱수를 나타내는 애너그램 쌍 찾기</t>
+  </si>
+  <si>
+    <t>CARE라는 단어의 각 글자를 1, 2, 9, 6이라는 숫자로 치환하면 1296 = 362이라는 제곱수가 됩니다. 그런데 동일한 치환 규칙을 CARE의 애너그램(anagram)인 RACE에 적용해보면, 역시 제곱수인 9216 = 962이 됩니다.
+(역주: 애너그램이란 철자 순서를 바꿔서 만든 단어를 말합니다) 
+위의 CARE와 RACE 같은 경우를 "제곱 애너그램 쌍"이라고 부르기로 하는데, 숫자로 치환할 때 맨 앞자리에는 0이 올 수 없고, 서로 다른 알파벳은 서로 다른 숫자에 대응되도록 합니다.
+16KB의 텍스트 파일 words.txt에 포함된 2000개 정도의 영어 단어 중에서 "제곱 애너그램 쌍"을 모두 찾으세요. 다만 거꾸로 해도 같은 단어가 되는 회문(palindrome)은 애너그램으로 치지 않습니다.
+이렇게 만들어진 제곱수 중 가장 큰 수는 얼마입니까?
+참고 : 만들어진 애너그램은 위의 텍스트 파일에 포함된 단어라야 합니다.</t>
+  </si>
+  <si>
+    <r>
+      <t>99</t>
+    </r>
+  </si>
+  <si>
+    <t>밑과 지수 형태로 나타낸 수 중 가장 큰 수 찾기</t>
+  </si>
+  <si>
+    <t>밑과 지수의 형태로 나타낸 2^11 와 3^7 같은 두 숫자를 비교하는 것은 어렵지 않습니다.
+ 아무 계산기나 갖고 두드려보면 2^11 = 2048 &lt; 3^7 = 2187 이라는 결과가 바로 나옵니다.
+하지만 632382^518061 &gt; 519432^525806 이 되는 것을 확인하기는 훨씬 더 어려운데, 그도 그럴 것이 두 숫자 모두 3백만자리가 넘는 수이기 때문입니다. 
+22KB 크기의 텍스트 파일 base_exp.txt에는 1천개의 숫자가 들어있는데, 한 줄에 하나씩이고 밑과 지수가 쉼표로 구분된 형태입니다. 이 중에서 가장 큰 숫자는 몇 번째 줄에 있는 숫자입니까? 
+참고 : 파일의 처음 두 줄은 위에 예를 들었던 두 숫자입니다.</t>
+  </si>
+  <si>
+    <r>
+      <t>100</t>
+    </r>
+  </si>
+  <si>
+    <t>두 개의 파란 공이 뽑힐 확률이 50%인 경우</t>
+  </si>
+  <si>
+    <t>파란 공 15개와 빨간 공 6개가 들어있는 상자에서 무작위로 두 개의 공을 꺼냈을 때, 두 개가 모두 파란색일 확률은 (15/21) × (14/20) = 1/2 입니다. 
+이렇게 무작위로 꺼낸 공 두 개가 모두 파란색일 확률이 정확히 50%가 되는 다음 번째 공의 배합은 파란 공 85개와 빨간 공 35개일 때입니다. 
+파란 공과 빨간 공을 합해서 모두 10^12 = 1,000,000,000,000 을 넘는 배합 중에서 위와 같은 확률을 가지면서 공의 수가 최소인 경우를 찾고, 이 때 파란 공은 모두 몇 개가 되는지 구하세요.</t>
+  </si>
+  <si>
+    <r>
+      <t>101</t>
+    </r>
+  </si>
+  <si>
+    <t>다항 함수의 BOP에서 나온 첫 오답의 총합은?</t>
+  </si>
+  <si>
+    <r>
+      <t>102</t>
+    </r>
+  </si>
+  <si>
+    <t>좌표평면의 원점을 지나는 삼각형의 개수는?</t>
+  </si>
+  <si>
+    <r>
+      <t>103</t>
+    </r>
+  </si>
+  <si>
+    <t>최적 특수합 집합의 원소를 한 문자열로 나열하면?</t>
+  </si>
+  <si>
+    <r>
+      <t>104</t>
+    </r>
+  </si>
+  <si>
+    <t>앞자리와 뒷자리가 모두 팬디지털인 첫 피보나치 항</t>
+  </si>
+  <si>
+    <r>
+      <t>105</t>
+    </r>
+  </si>
+  <si>
+    <t>특수합 집합의 원소의 총합</t>
+  </si>
+  <si>
+    <r>
+      <t>106</t>
+    </r>
+  </si>
+  <si>
+    <t>규칙에 위배되는 예비 특수합 집합의 수</t>
+  </si>
+  <si>
+    <r>
+      <t>107</t>
+    </r>
+  </si>
+  <si>
+    <t>최소 그래프</t>
+  </si>
+  <si>
+    <r>
+      <t>108</t>
+    </r>
+  </si>
+  <si>
+    <t>디오판투스 항등식</t>
+  </si>
+  <si>
+    <r>
+      <t>109</t>
+    </r>
+  </si>
+  <si>
+    <t>다트 문제</t>
+  </si>
+  <si>
+    <r>
+      <t>110</t>
+    </r>
+  </si>
+  <si>
+    <t>디오판투스 항등식 2</t>
+  </si>
+  <si>
+    <r>
+      <t>111</t>
+    </r>
+  </si>
+  <si>
+    <t>특정한 수가 반복될 때 소수</t>
+  </si>
+  <si>
+    <r>
+      <t>112</t>
+    </r>
+  </si>
+  <si>
+    <t>오락가락수</t>
+  </si>
+  <si>
+    <r>
+      <t>113</t>
+    </r>
+  </si>
+  <si>
+    <t>오락가락수가 아닌 수</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
@@ -750,6 +1944,18 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11.0"/>
       <name val="맑은 고딕"/>
       <color theme="1"/>
@@ -957,9 +2163,7 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -974,25 +2178,33 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -1007,7 +2219,9 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -1022,7 +2236,9 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="double">
@@ -1037,13 +2253,17 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <top style="thin">
@@ -1052,7 +2272,9 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -1106,7 +2328,7 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1142,6 +2364,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1462,472 +2693,1310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.750000" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.500000" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.75500011" customWidth="1" outlineLevel="0"/>
     <col min="2" max="2" width="72.37999725" customWidth="1" outlineLevel="0"/>
-    <col min="3" max="3" style="8" width="119.00499725" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" style="5" width="119.00499725" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A19" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A24" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A25" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A27" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A28" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="9" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A29" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="9" t="s">
         <v>85</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A30" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A31" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" ht="13.500000" customHeight="1">
+      <c r="A32" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A33" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A34" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>100</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A35" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="9" t="s">
         <v>103</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A36" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="9" t="s">
         <v>106</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A37" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A38" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="9" t="s">
         <v>112</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A39" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="9" t="s">
         <v>115</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A40" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="9" t="s">
         <v>118</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.750000" customHeight="1">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A41" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="9" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>122</v>
       </c>
+    </row>
+    <row r="42" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A42" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A43" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A44" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A45" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A46" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A47" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A48" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A49" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A50" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A51" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A52" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A53" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A54" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A55" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A56" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A57" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A58" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A59" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A60" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A61" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A62" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A63" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A64" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A65" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A66" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A67" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A68" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A69" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A70" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A71" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A72" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A73" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A74" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A75" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A76" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A77" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A78" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A79" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A80" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A81" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A82" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A83" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A84" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A85" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A86" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A87" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A88" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A89" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A90" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A91" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A92" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A93" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A94" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A95" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A96" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A97" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A98" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A99" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A100" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A101" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A102" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A103" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A104" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C104" s="9"/>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A105" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C105" s="9"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A106" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C106" s="9"/>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A107" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C107" s="9"/>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A108" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C108" s="9"/>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A109" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="C109" s="9"/>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A110" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A111" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C111" s="9"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A112" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C112" s="9"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A113" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" ht="13.500000" customHeight="1">
+      <c r="A114" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C114" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>